<commit_message>
tables to for lab3
</commit_message>
<xml_diff>
--- a/Lab3/3a_async_tabela.xlsx
+++ b/Lab3/3a_async_tabela.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\luknw\studia\03_semestr\Techniki cyfrowe\cyfrowa\Lab3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Dropbox\Studia\Technika Cyfrowa\cyfrowa\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,30 +24,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>X2</t>
-  </si>
-  <si>
-    <t>X4</t>
-  </si>
-  <si>
-    <t>X6</t>
-  </si>
-  <si>
-    <t>X8</t>
-  </si>
-  <si>
-    <t>poprz. stan</t>
-  </si>
-  <si>
-    <t>zabroniony</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+  <si>
+    <t>Wnioski: Bramka zrealizowana na NORach zachowuje się identycznie jak NANDowa z tą różnicą, że na NORach stan poprzedni jest przyjmowany dla (0,0) a na NANDach - dla (1,1) =&gt; bramka NORowa jest bardziej energooszczędna</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Karnaugh dla NORa</t>
+  </si>
+  <si>
+    <t>Q(n) (NOR)</t>
+  </si>
+  <si>
+    <t>Q(n) (NAND)</t>
+  </si>
+  <si>
+    <t>Q(n-1)</t>
+  </si>
+  <si>
+    <t>zab</t>
+  </si>
+  <si>
+    <t>Q(n-1)\RS</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Karnaugh dla NANDa</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>S + Q(n-1)R'S'</t>
+  </si>
+  <si>
+    <t>R'+Q(n-1)RS</t>
   </si>
 </sst>
 </file>
@@ -108,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -120,9 +153,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -138,9 +189,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -178,7 +229,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -250,7 +301,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -400,42 +451,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="6" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E1" s="4"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -446,20 +492,14 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E2" s="4"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -470,20 +510,14 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E3" s="4"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -494,20 +528,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E4" s="4"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -518,63 +546,939 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E5" s="4"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="8"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="8"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" s="8"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+      <c r="N48" s="6"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="6"/>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="6"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="6"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
+      <c r="N54" s="6"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="6"/>
+      <c r="M55" s="6"/>
+      <c r="N55" s="6"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
+      <c r="L56" s="6"/>
+      <c r="M56" s="6"/>
+      <c r="N56" s="6"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="6"/>
+      <c r="K57" s="6"/>
+      <c r="L57" s="6"/>
+      <c r="M57" s="6"/>
+      <c r="N57" s="6"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A58" s="6"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6"/>
+      <c r="K58" s="6"/>
+      <c r="L58" s="6"/>
+      <c r="M58" s="6"/>
+      <c r="N58" s="6"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A59" s="6"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+      <c r="L59" s="6"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
3A fine and dandy
</commit_message>
<xml_diff>
--- a/Lab3/3a_async_tabela.xlsx
+++ b/Lab3/3a_async_tabela.xlsx
@@ -87,8 +87,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -141,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -170,6 +179,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,26 +471,26 @@
   <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="16" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="4"/>
@@ -649,35 +666,35 @@
       <c r="N11" s="6"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="11"/>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="15" t="s">
         <v>14</v>
       </c>
       <c r="L12" s="8"/>
@@ -685,7 +702,7 @@
       <c r="N12" s="6"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="14" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="12" t="s">
@@ -701,7 +718,7 @@
         <v>9</v>
       </c>
       <c r="F13" s="11"/>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="14" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="12" t="s">
@@ -721,7 +738,7 @@
       <c r="N13" s="6"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -737,7 +754,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="11"/>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="14" t="s">
         <v>10</v>
       </c>
       <c r="H14" s="12" t="s">

</xml_diff>

<commit_message>
Michelangelo couldn't have done 3A better than it's done now.
</commit_message>
<xml_diff>
--- a/Lab3/3a_async_tabela.xlsx
+++ b/Lab3/3a_async_tabela.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Dropbox\Studia\Technika Cyfrowa\cyfrowa\Lab3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\luknw\studia\03_semestr\TC\cyfrowa\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
-  <si>
-    <t>Wnioski: Bramka zrealizowana na NORach zachowuje się identycznie jak NANDowa z tą różnicą, że na NORach stan poprzedni jest przyjmowany dla (0,0) a na NANDach - dla (1,1) =&gt; bramka NORowa jest bardziej energooszczędna</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>R</t>
   </si>
@@ -35,9 +32,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>Karnaugh dla NORa</t>
-  </si>
-  <si>
     <t>Q(n) (NOR)</t>
   </si>
   <si>
@@ -50,9 +44,6 @@
     <t>zab</t>
   </si>
   <si>
-    <t>Q(n-1)\RS</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -71,23 +62,256 @@
     <t>10</t>
   </si>
   <si>
-    <t>Karnaugh dla NANDa</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
-    <t>S + Q(n-1)R'S'</t>
-  </si>
-  <si>
-    <t>R'+Q(n-1)RS</t>
+    <t>Q(n-1)\SR</t>
+  </si>
+  <si>
+    <t>NOR</t>
+  </si>
+  <si>
+    <t>NAND</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Q(n) = S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R'Q(n-1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = (S nor (R nor Q'(n-1)))'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Q'(n) = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S'Q'(n-1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = (R nor (S nor Q(n-1)))'</t>
+    </r>
+  </si>
+  <si>
+    <t>Q(n) = R nor (S nor Q(n-1))</t>
+  </si>
+  <si>
+    <t>Q'(n) = S nor (R nor Q'(n-1))</t>
+  </si>
+  <si>
+    <t>Po zanegowaniu stronami obu równań:</t>
+  </si>
+  <si>
+    <t>Q(n) = R' nor (S' nor Q(n-1))</t>
+  </si>
+  <si>
+    <t>Q'(n) = S' nor (R' nor Q'(n-1))</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Q(n) = S'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RQ(n-1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = S nand (R nand Q(n-1))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Q'(n) = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SQ'(n-1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = R nand (S nand Q'(n-1))</t>
+    </r>
+  </si>
+  <si>
+    <t>Zauważmy, że możemy przekształcić inaczej:</t>
+  </si>
+  <si>
+    <t>Q(n) = S' + RQ(n-1) = (S' nor (R' nor Q'(n-1)))'</t>
+  </si>
+  <si>
+    <t>Q'(n) = R' + SQ'(n-1) = (R' nor (S' nor Q(n-1)))'</t>
+  </si>
+  <si>
+    <t>Po zanegowaniu stronami:</t>
+  </si>
+  <si>
+    <t>Forma analogiczna jak dla bramek nor,</t>
+  </si>
+  <si>
+    <t>jednak z zanegowanymi wejściami.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,16 +329,65 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -146,11 +419,150 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -171,9 +583,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -181,16 +590,69 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -206,9 +668,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -246,7 +708,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -318,7 +780,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -468,556 +930,545 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N59"/>
+  <dimension ref="A3:Q59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
+      <c r="E3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="10"/>
+      <c r="M3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="10"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="M6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
+      <c r="N6" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="P6" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q7" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
       <c r="L9" s="8"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="11"/>
+      <c r="M9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
       <c r="L10" s="8"/>
-      <c r="M10" s="6"/>
+      <c r="M10" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="N10" s="6"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
       <c r="L11" s="8"/>
-      <c r="M11" s="6"/>
       <c r="N11" s="6"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="8"/>
-      <c r="M12" s="6"/>
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="G12" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="N12" s="6"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="L13" s="8"/>
-      <c r="M13" s="6"/>
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="G13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="N13" s="6"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>9</v>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F14" s="16"/>
+      <c r="G14" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="L14" s="8"/>
-      <c r="M14" s="6"/>
+      <c r="M14" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="N14" s="6"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F15" s="10"/>
       <c r="L15" s="8"/>
-      <c r="M15" s="6"/>
+      <c r="M15" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="N15" s="6"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F16" s="10"/>
       <c r="L16" s="8"/>
-      <c r="M16" s="6"/>
+      <c r="M16" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="N16" s="6"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
       <c r="L17" s="8"/>
-      <c r="M17" s="6"/>
+      <c r="M17" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="N17" s="6"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
       <c r="L18" s="8"/>
-      <c r="M18" s="6"/>
+      <c r="M18" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="N18" s="6"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
       <c r="L19" s="8"/>
-      <c r="M19" s="6"/>
+      <c r="M19" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="N19" s="6"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
       <c r="L20" s="8"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
       <c r="L21" s="8"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
       <c r="L22" s="8"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
       <c r="L23" s="8"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
       <c r="L24" s="8"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
       <c r="L25" s="8"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
       <c r="L26" s="8"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
       <c r="L27" s="8"/>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
       <c r="L28" s="8"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
       <c r="L29" s="8"/>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -1033,7 +1484,7 @@
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -1049,7 +1500,7 @@
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1065,7 +1516,7 @@
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -1081,7 +1532,7 @@
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1097,7 +1548,7 @@
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -1113,7 +1564,7 @@
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1129,7 +1580,7 @@
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -1145,7 +1596,7 @@
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1161,7 +1612,7 @@
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -1177,7 +1628,7 @@
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -1193,7 +1644,7 @@
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -1209,7 +1660,7 @@
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -1225,7 +1676,7 @@
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1241,7 +1692,7 @@
       <c r="M43" s="6"/>
       <c r="N43" s="6"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -1257,7 +1708,7 @@
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -1273,7 +1724,7 @@
       <c r="M45" s="6"/>
       <c r="N45" s="6"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -1289,7 +1740,7 @@
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -1305,7 +1756,7 @@
       <c r="M47" s="6"/>
       <c r="N47" s="6"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -1321,7 +1772,7 @@
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -1337,7 +1788,7 @@
       <c r="M49" s="6"/>
       <c r="N49" s="6"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -1353,7 +1804,7 @@
       <c r="M50" s="6"/>
       <c r="N50" s="6"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -1369,7 +1820,7 @@
       <c r="M51" s="6"/>
       <c r="N51" s="6"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -1385,7 +1836,7 @@
       <c r="M52" s="6"/>
       <c r="N52" s="6"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -1401,7 +1852,7 @@
       <c r="M53" s="6"/>
       <c r="N53" s="6"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -1417,7 +1868,7 @@
       <c r="M54" s="6"/>
       <c r="N54" s="6"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -1433,7 +1884,7 @@
       <c r="M55" s="6"/>
       <c r="N55" s="6"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -1449,7 +1900,7 @@
       <c r="M56" s="6"/>
       <c r="N56" s="6"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -1465,7 +1916,7 @@
       <c r="M57" s="6"/>
       <c r="N57" s="6"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -1481,7 +1932,7 @@
       <c r="M58" s="6"/>
       <c r="N58" s="6"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>

</xml_diff>